<commit_message>
Final presentation, search posts
Added final presentation for the documents, changed look for posts in
search results
</commit_message>
<xml_diff>
--- a/Documentation/Requirements.xlsx
+++ b/Documentation/Requirements.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25580" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -690,8 +690,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -743,13 +743,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008000"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -782,7 +782,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -792,27 +792,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1141,19 +1143,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="37.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="37.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="3" max="5" width="70.83203125" customWidth="1"/>
-    <col min="6" max="6" width="89.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="82.375" customWidth="1"/>
+    <col min="4" max="5" width="70.875" customWidth="1"/>
+    <col min="6" max="6" width="89.875" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1301,7 +1302,7 @@
       <c r="F7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -1322,7 +1323,7 @@
       <c r="F8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
@@ -1343,7 +1344,7 @@
       <c r="F9" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
@@ -1364,7 +1365,7 @@
       <c r="F10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
@@ -1385,7 +1386,7 @@
       <c r="F11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
@@ -1427,7 +1428,7 @@
       <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
@@ -1448,7 +1449,7 @@
       <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
@@ -1511,7 +1512,7 @@
       <c r="F17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
@@ -1553,7 +1554,7 @@
       <c r="F19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
@@ -1595,7 +1596,7 @@
       <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
@@ -1616,7 +1617,7 @@
       <c r="F22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
@@ -1637,7 +1638,7 @@
       <c r="F23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
@@ -1742,7 +1743,7 @@
       <c r="F28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
@@ -1889,6 +1890,7 @@
       <c r="F35" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
@@ -1930,7 +1932,7 @@
       <c r="F37" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G37" s="1"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
@@ -1993,7 +1995,7 @@
       <c r="F40" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G40" s="1"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
@@ -2014,7 +2016,7 @@
       <c r="F41" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G41" s="1"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
@@ -2035,7 +2037,7 @@
       <c r="F42" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
@@ -2056,6 +2058,7 @@
       <c r="F43" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
@@ -2118,7 +2121,7 @@
       <c r="F46" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="G46" s="6"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
@@ -2143,7 +2146,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>